<commit_message>
Add user stories testing in testing.md
</commit_message>
<xml_diff>
--- a/readme-testing-images/User-Stories.xlsx
+++ b/readme-testing-images/User-Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paola\Desktop\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E8CDAF-900D-4435-BB10-EDD4F8CCCE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B7CD0-A2FD-46B1-A896-0EFDF30A9E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1ECFAA28-1FEE-4995-A1D8-518CF20934EA}"/>
   </bookViews>
@@ -127,9 +127,6 @@
 </t>
   </si>
   <si>
-    <t>so that I can view the results ordered by price, popularity, date (able to see newest items).</t>
-  </si>
-  <si>
     <t xml:space="preserve"> I want to be able to search the available cupcakes by name and description </t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>so that they can be used for a future purchase.</t>
   </si>
   <si>
-    <t>I want to be able to save my payment information when creating an order</t>
-  </si>
-  <si>
     <t xml:space="preserve">I want to view an order summary and confirmation after checkout </t>
   </si>
   <si>
@@ -233,6 +227,12 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>so that I can view the results ordered by price, date, name and category.</t>
+  </si>
+  <si>
+    <t>I want to be able to save my delivery information when creating an order</t>
   </si>
 </sst>
 </file>
@@ -335,18 +335,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -354,6 +342,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58793A07-E161-4414-8FF3-37E169DE9C19}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,12 +704,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -722,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -736,16 +736,16 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -758,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -786,16 +786,16 @@
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -808,7 +808,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -836,7 +836,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -850,29 +850,29 @@
         <v>28</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -880,13 +880,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -894,35 +894,35 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -930,13 +930,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -944,13 +944,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,13 +958,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -972,13 +972,13 @@
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -986,13 +986,13 @@
         <v>18</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1000,35 +1000,35 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1036,74 +1036,74 @@
         <v>18</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>